<commit_message>
ADD DICTIONNARY AND HASHTAG UNIQUENESS
</commit_message>
<xml_diff>
--- a/src/blizzfact.xlsx
+++ b/src/blizzfact.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="124">
   <si>
     <t>URL of the post</t>
   </si>
@@ -123,6 +123,15 @@
     <t>In what position it got featured?</t>
   </si>
   <si>
+    <t>List of only unique (most media-related) hashtags used in the caption</t>
+  </si>
+  <si>
+    <t>Number of unique (most media-related) hashtags used in the post</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hashtag Uniqueness Coefficient </t>
+  </si>
+  <si>
     <t>0-10k hashtags</t>
   </si>
   <si>
@@ -154,6 +163,18 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>Amount of the same hashtags used in the caption from previous post caption</t>
+  </si>
+  <si>
+    <t>Number of new words being used in the post caption in comparison from previous caption (eliminating emojis,tags,hashtags, and words are not case sensitive)</t>
+  </si>
+  <si>
+    <t>Percentage of the same words being used on second post (elimination of emojis, tags and hashtags being used and words are not case sensitive) (Caption dictonary uniqueness)</t>
+  </si>
+  <si>
+    <t>Uniqueness of the caption based on overall data (based on all posts captions)</t>
   </si>
   <si>
     <t>https://www.instagram.com/p/BnFZRcOAo3K/?taken-by=blizzfact</t>
@@ -167,7 +188,7 @@
 #useyourbrain #factsz #goodword #truefact #youknowit #themoreyouknow #keepit100 #payattention #humbleyourself #believing #learn #liveandlearn #imjustsaying</t>
   </si>
   <si>
-    <t>goodword,truefact,factsz,keepit100,imjustsaying,liveandlearn,themoreyouknow,payattention,humbleyourself,useyourbrain,learn,believing,youknowit</t>
+    <t>themoreyouknow,humbleyourself,imjustsaying,liveandlearn,payattention,useyourbrain,keepit100,believing,youknowit,goodword,truefact,factsz,learn</t>
   </si>
   <si>
     <t>✌✌👇👆</t>
@@ -218,6 +239,9 @@
     <t>NO</t>
   </si>
   <si>
+    <t>themoreyouknow,humbleyourself,imjustsaying,liveandlearn,payattention,useyourbrain,keepit100,believing,youknowit,learn</t>
+  </si>
+  <si>
     <t>factsz</t>
   </si>
   <si>
@@ -234,6 +258,151 @@
   </si>
   <si>
     <t>learn</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/BnE2BfagCXm/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>Comment UNKNOWNFACTS without getting interrupted 👇
+✌️
+@blizzfact
+@blizzfact
+👇
+#goodword #neverforgetthat #factss #factsz #sayingsandquotes #dontthinkaboutit #factset #realness #lessonslearned</t>
+  </si>
+  <si>
+    <t>dontthinkaboutit,sayingsandquotes,neverforgetthat,lessonslearned,goodword,realness,factset,factss,factsz</t>
+  </si>
+  <si>
+    <t>👇✌👇</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/273503011/eiffel-tower-paris-tennessee/</t>
+  </si>
+  <si>
+    <t>Wednesday</t>
+  </si>
+  <si>
+    <t>gallery</t>
+  </si>
+  <si>
+    <t>1856846543345165798</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/115055346b956fe6603a240e95be9689/5C150078/t51.2885-15/e35/39531967_251483822370127_642556854425092096_n.jpg,https://scontent-mrs1-1.cdninstagram.com/vp/4453ffbcbab64c391e3f2aac30fdf4bb/5C2E4DAB/t51.2885-15/e35/39748013_1482343511866045_3356968849692950528_n.jpg,https://scontent-mrs1-1.cdninstagram.com/vp/876be58bd938647831ceb1287eedf3bd/5C25FE8D/t51.2885-15/e35/39341845_216685952539450_609343026216566784_n.jpg,https://scontent-mrs1-1.cdninstagram.com/vp/2cd49678aa6be2eed7fa3d39823ff77e/5C011BEB/t51.2885-15/e35/39894924_294277514691241_5045292915765542912_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/galleries/gallery_1856846543345165798/</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/galleries/gallery_1856846543345165798/39531967_251483822370127_642556854425092096_n.jpg,./outputs/blizzfact/galleries/gallery_1856846543345165798/39748013_1482343511866045_3356968849692950528_n.jpg,./outputs/blizzfact/galleries/gallery_1856846543345165798/39341845_216685952539450_609343026216566784_n.jpg,./outputs/blizzfact/galleries/gallery_1856846543345165798/39894924_294277514691241_5045292915765542912_n.jpg</t>
+  </si>
+  <si>
+    <t>39531967_251483822370127_642556854425092096_n.jpg,39748013_1482343511866045_3356968849692950528_n.jpg,39341845_216685952539450_609343026216566784_n.jpg,39894924_294277514691241_5045292915765542912_n.jpg</t>
+  </si>
+  <si>
+    <t>1080x1080,1080x1080,1080x1080,1080x1080</t>
+  </si>
+  <si>
+    <t>320.972,635.377,531.662,483.308</t>
+  </si>
+  <si>
+    <t>Eiffel Tower (Paris, Tennessee)</t>
+  </si>
+  <si>
+    <t>273503011</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>dontthinkaboutit,sayingsandquotes,neverforgetthat,realness,factset,factss</t>
+  </si>
+  <si>
+    <t>factsz,factset</t>
+  </si>
+  <si>
+    <t>dontthinkaboutit,neverforgetthat</t>
+  </si>
+  <si>
+    <t>factss</t>
+  </si>
+  <si>
+    <t>goodword</t>
+  </si>
+  <si>
+    <t>sayingsandquotes</t>
+  </si>
+  <si>
+    <t>lessonslearned,realness</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/BnBsvtwgbXV/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>Didn't know prostitution is legal in Australia 😛
+Follow: @blizzfact 😻
+👇
+TURN ON POST NOTIFICATIONS!
+👆
+#factsonfacts #realshitdoe #stilltrue #factssss #complicatedlife #goodword #interestingfacts #realshitonly #powerfull #knowledgeispower #knowledge #truths #truedat #keepitreal #lessonslearned #mindblowing #itiswhatitis #sotrue #lessonlearned #funfact #akward #positivethoughts #pretend #mindgames #quotesgram #truefact #randomness #beliveinyourself</t>
+  </si>
+  <si>
+    <t>interestingfacts,positivethoughts,beliveinyourself,knowledgeispower,complicatedlife,lessonslearned,lessonlearned,realshitonly,factsonfacts,itiswhatitis,realshitdoe,mindblowing,randomness,quotesgram,keepitreal,knowledge,stilltrue,powerfull,mindgames,goodword,truefact,factssss,pretend,truedat,funfact,sotrue,akward,truths</t>
+  </si>
+  <si>
+    <t>😛😻👇👆</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/683630/musee-du-louvre/</t>
+  </si>
+  <si>
+    <t>Tuesday</t>
+  </si>
+  <si>
+    <t>1855961314447439317</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/65c3869026abcbb0693cc97a69c7f8c5/5C345C43/t51.2885-15/e35/37167064_2131363020458347_9145305409907589120_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/37167064_2131363020458347_9145305409907589120_n.jpg</t>
+  </si>
+  <si>
+    <t>37167064_2131363020458347_9145305409907589120_n.jpg</t>
+  </si>
+  <si>
+    <t>614.537</t>
+  </si>
+  <si>
+    <t>Musée du Louvre</t>
+  </si>
+  <si>
+    <t>683630</t>
+  </si>
+  <si>
+    <t>interestingfacts,positivethoughts,beliveinyourself,knowledgeispower,complicatedlife,lessonlearned,realshitonly,factsonfacts,itiswhatitis,realshitdoe,mindblowing,randomness,quotesgram,keepitreal,knowledge,stilltrue,powerfull,mindgames,factssss,pretend,truedat,funfact,sotrue,akward,truths</t>
+  </si>
+  <si>
+    <t>realshitonly,complicatedlife</t>
+  </si>
+  <si>
+    <t>realshitdoe,factssss</t>
+  </si>
+  <si>
+    <t>stilltrue,factsonfacts</t>
+  </si>
+  <si>
+    <t>interestingfacts,akward,mindgames</t>
+  </si>
+  <si>
+    <t>lessonslearned,pretend,truefact,powerfull,mindblowing,beliveinyourself,truedat</t>
+  </si>
+  <si>
+    <t>randomness,lessonlearned,quotesgram,itiswhatitis,positivethoughts,knowledgeispower</t>
+  </si>
+  <si>
+    <t>knowledge,sotrue</t>
   </si>
 </sst>
 </file>
@@ -261,7 +430,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="19">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,12 +530,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE0BC5D"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA6F914"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -398,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -446,9 +609,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="17" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -754,13 +914,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BY2"/>
+  <dimension ref="A1:BY4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="40" customHeight="1"/>
   <cols>
-    <col min="1" max="24" width="50.7109375" customWidth="1"/>
+    <col min="1" max="101" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:77" ht="40" customHeight="1">
@@ -824,95 +984,107 @@
       <c r="T1" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="U1" s="17" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>22</v>
+      <c r="U1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="W1" s="16" t="s">
+        <v>37</v>
       </c>
       <c r="X1" s="15" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="Y1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AC1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD1" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AI1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ1" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="AK1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AL1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AM1" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="AN1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AO1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AP1" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="16" t="s">
+      <c r="AQ1" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="AR1" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="AS1" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="AA1" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="AB1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AC1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AD1" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AF1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AG1" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="AH1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AJ1" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="AK1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AL1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AM1" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="AN1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AO1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AP1" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="AR1" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="AS1" s="15" t="s">
-        <v>42</v>
-      </c>
       <c r="AT1" s="16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AU1" s="16" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="AV1" s="15" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AW1" s="16" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="AX1" s="16" t="s">
-        <v>45</v>
+        <v>48</v>
+      </c>
+      <c r="AY1" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="AZ1" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="BA1" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="BB1" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="BU1" s="13" t="s">
         <v>16</v>
@@ -931,157 +1103,505 @@
       </c>
     </row>
     <row r="2" spans="1:77" ht="40" customHeight="1">
-      <c r="A2" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B2" s="18" t="s">
+      <c r="A2" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="17" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="17" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" s="17">
+        <v>970</v>
+      </c>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17">
+        <v>10</v>
+      </c>
+      <c r="L2" s="18">
+        <v>0.07863906275076232</v>
+      </c>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17">
+        <v>0</v>
+      </c>
+      <c r="O2" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P2" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q2" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="R2" s="19">
+        <v>43342</v>
+      </c>
+      <c r="S2" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="C2" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="18" t="s">
+      <c r="T2" s="17">
+        <v>13</v>
+      </c>
+      <c r="U2" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="V2" s="17">
+        <v>10</v>
+      </c>
+      <c r="W2" s="18">
+        <v>0.7692307692307693</v>
+      </c>
+      <c r="X2" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="Y2" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z2" s="18">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="AA2" s="17"/>
+      <c r="AB2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="AH2" s="17">
+        <v>2</v>
+      </c>
+      <c r="AI2" s="18">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="AJ2" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK2" s="17">
+        <v>2</v>
+      </c>
+      <c r="AL2" s="18">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="AM2" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN2" s="17">
+        <v>4</v>
+      </c>
+      <c r="AO2" s="18">
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="AP2" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ2" s="17">
+        <v>3</v>
+      </c>
+      <c r="AR2" s="18">
+        <v>0.2307692307692308</v>
+      </c>
+      <c r="AS2" s="17"/>
+      <c r="AT2" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="AW2" s="17">
+        <v>1</v>
+      </c>
+      <c r="AX2" s="18">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="AY2" s="17">
+        <v>2</v>
+      </c>
+      <c r="AZ2" s="17">
+        <v>12</v>
+      </c>
+      <c r="BA2" s="18">
+        <v>0</v>
+      </c>
+      <c r="BB2" s="18">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="BU2" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="E2" s="18" t="s">
-        <v>58</v>
-      </c>
-      <c r="F2" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>60</v>
-      </c>
-      <c r="H2" s="18" t="s">
+      <c r="BV2" s="17" t="s">
+        <v>69</v>
+      </c>
+      <c r="BW2" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="BX2" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="BY2" s="17"/>
+    </row>
+    <row r="3" spans="1:77" ht="40" customHeight="1">
+      <c r="A3" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>88</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>90</v>
+      </c>
+      <c r="G3" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="17">
+        <v>615</v>
+      </c>
+      <c r="J3" s="17"/>
+      <c r="K3" s="17">
+        <v>2</v>
+      </c>
+      <c r="L3" s="18">
+        <v>0.04951051195634729</v>
+      </c>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17">
+        <v>0</v>
+      </c>
+      <c r="O3" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="I2" s="18">
-        <v>819</v>
-      </c>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18">
+      <c r="P3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="R3" s="19">
+        <v>43341</v>
+      </c>
+      <c r="S3" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="T3" s="17">
         <v>9</v>
       </c>
-      <c r="L2" s="19">
-        <v>0.06645264847512039</v>
-      </c>
-      <c r="M2" s="18"/>
-      <c r="N2" s="18">
-        <v>0</v>
-      </c>
-      <c r="O2" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="P2" s="18">
+      <c r="U3" s="17" t="s">
+        <v>96</v>
+      </c>
+      <c r="V3" s="17">
+        <v>6</v>
+      </c>
+      <c r="W3" s="18">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="Y3" s="17">
+        <v>2</v>
+      </c>
+      <c r="Z3" s="18">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="AA3" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="AB3" s="17">
+        <v>2</v>
+      </c>
+      <c r="AC3" s="18">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="AD3" s="17" t="s">
+        <v>99</v>
+      </c>
+      <c r="AE3" s="17">
         <v>1</v>
       </c>
-      <c r="Q2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="R2" s="20">
-        <v>43342</v>
-      </c>
-      <c r="S2" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="18">
-        <v>13</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="V2" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="W2" s="18"/>
-      <c r="X2" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y2" s="18">
+      <c r="AF3" s="18">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="AG3" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH3" s="17">
         <v>1</v>
       </c>
-      <c r="Z2" s="19">
-        <v>0.07692307692307693</v>
-      </c>
-      <c r="AA2" s="18"/>
-      <c r="AB2" s="18">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="18"/>
-      <c r="AE2" s="18">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="AH2" s="18">
+      <c r="AI3" s="18">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="AJ3" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="AK3" s="17">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="18">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="AM3" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="AN3" s="17">
         <v>2</v>
       </c>
-      <c r="AI2" s="19">
-        <v>0.1538461538461539</v>
-      </c>
-      <c r="AJ2" s="18" t="s">
+      <c r="AO3" s="18">
+        <v>0.2222222222222222</v>
+      </c>
+      <c r="AP3" s="17"/>
+      <c r="AQ3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="17"/>
+      <c r="AT3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="17"/>
+      <c r="AW3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="17">
+        <v>2</v>
+      </c>
+      <c r="AZ3" s="17">
+        <v>5</v>
+      </c>
+      <c r="BA3" s="18">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="18">
+        <v>1</v>
+      </c>
+      <c r="BU3" s="17" t="s">
+        <v>83</v>
+      </c>
+      <c r="BV3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="BW3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="BX3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="BY3" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:77" ht="40" customHeight="1">
+      <c r="A4" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>110</v>
+      </c>
+      <c r="D4" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="G4" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="AK2" s="18">
+      <c r="H4" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="17">
+        <v>767</v>
+      </c>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17">
+        <v>0</v>
+      </c>
+      <c r="L4" s="18">
+        <v>0.06154710319370887</v>
+      </c>
+      <c r="M4" s="17"/>
+      <c r="N4" s="17">
+        <v>0</v>
+      </c>
+      <c r="O4" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="R4" s="19">
+        <v>43340</v>
+      </c>
+      <c r="S4" s="17" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" s="17">
+        <v>28</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="V4" s="17">
+        <v>25</v>
+      </c>
+      <c r="W4" s="18">
+        <v>0.8928571428571429</v>
+      </c>
+      <c r="X4" s="17" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y4" s="17">
         <v>2</v>
       </c>
-      <c r="AL2" s="19">
-        <v>0.1538461538461539</v>
-      </c>
-      <c r="AM2" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="AN2" s="18">
-        <v>4</v>
-      </c>
-      <c r="AO2" s="19">
-        <v>0.3076923076923077</v>
-      </c>
-      <c r="AP2" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ2" s="18">
+      <c r="Z4" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="AA4" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="AB4" s="17">
+        <v>2</v>
+      </c>
+      <c r="AC4" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="AD4" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="AE4" s="17">
+        <v>2</v>
+      </c>
+      <c r="AF4" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="AG4" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="AH4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AI4" s="18">
+        <v>0.04</v>
+      </c>
+      <c r="AJ4" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="AK4" s="17">
         <v>3</v>
       </c>
-      <c r="AR2" s="19">
-        <v>0.2307692307692308</v>
-      </c>
-      <c r="AS2" s="18"/>
-      <c r="AT2" s="18">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="19">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW2" s="18">
-        <v>1</v>
-      </c>
-      <c r="AX2" s="19">
-        <v>0.07692307692307693</v>
-      </c>
-      <c r="BU2" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="BV2" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="BW2" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="BX2" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="BY2" s="18"/>
+      <c r="AL4" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="AM4" s="17" t="s">
+        <v>121</v>
+      </c>
+      <c r="AN4" s="17">
+        <v>7</v>
+      </c>
+      <c r="AO4" s="18">
+        <v>0.28</v>
+      </c>
+      <c r="AP4" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="AQ4" s="17">
+        <v>6</v>
+      </c>
+      <c r="AR4" s="18">
+        <v>0.24</v>
+      </c>
+      <c r="AS4" s="17"/>
+      <c r="AT4" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="AW4" s="17">
+        <v>2</v>
+      </c>
+      <c r="AX4" s="18">
+        <v>0.08</v>
+      </c>
+      <c r="AY4" s="17"/>
+      <c r="AZ4" s="17"/>
+      <c r="BA4" s="18"/>
+      <c r="BB4" s="18">
+        <v>0.5833333333333334</v>
+      </c>
+      <c r="BU4" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="BV4" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="BW4" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="BX4" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="BY4" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new lines added in sheet n°2
</commit_message>
<xml_diff>
--- a/src/blizzfact.xlsx
+++ b/src/blizzfact.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="301">
   <si>
     <t>URL of the post</t>
   </si>
@@ -175,6 +176,89 @@
   </si>
   <si>
     <t>Uniqueness of the caption based on overall data (based on all posts captions)</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/BnH-NAoAvHO/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>Such a lier. Any Trump haters? 👍
+Follow: @blizzfact before your friends did 😻
+👇
+TURN ON POST NOTIFICATIONS!
+👆
+#realtalktho #whenitsreal #questionmark #lifeslessons #tellhim #factsb #sayingsandquotes #itiswhatitis #truedat #wordoftheday #educateyourself #factsoflife #beliveinyourself #betrue #wikipedia #facts #truths #funnybuttrue #realness #akward #liveandlearn #imjustsaying #funfact #positivemind</t>
+  </si>
+  <si>
+    <t>sayingsandquotes,beliveinyourself,educateyourself,funnybuttrue,positivemind,imjustsaying,wordoftheday,lifeslessons,itiswhatitis,liveandlearn,questionmark,whenitsreal,factsoflife,realtalktho,wikipedia,realness,tellhim,funfact,truedat,factsb,akward,truths,betrue,facts</t>
+  </si>
+  <si>
+    <t>👍😻👇👆</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/488284047/strip-vegas/</t>
+  </si>
+  <si>
+    <t>Friday</t>
+  </si>
+  <si>
+    <t>August</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>blizzfact</t>
+  </si>
+  <si>
+    <t>1857726944221786574</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/61b9da1a8c7239063e96c464694ce068/5C378EF2/t51.2885-15/e35/40191888_908051792729024_5154282048818511872_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/40191888_908051792729024_5154282048818511872_n.jpg</t>
+  </si>
+  <si>
+    <t>40191888_908051792729024_5154282048818511872_n.jpg</t>
+  </si>
+  <si>
+    <t>1080x1080</t>
+  </si>
+  <si>
+    <t>484.226</t>
+  </si>
+  <si>
+    <t>Strip Vegas</t>
+  </si>
+  <si>
+    <t>488284047</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>lifeslessons,questionmark,realtalktho,wikipedia,facts</t>
+  </si>
+  <si>
+    <t>tellhim,factsb,whenitsreal</t>
+  </si>
+  <si>
+    <t>lifeslessons,realtalktho</t>
+  </si>
+  <si>
+    <t>funnybuttrue,akward,sayingsandquotes,wikipedia,questionmark</t>
+  </si>
+  <si>
+    <t>truths,imjustsaying,beliveinyourself,factsoflife,realness,truedat</t>
+  </si>
+  <si>
+    <t>positivemind,wordoftheday,itiswhatitis,liveandlearn,funfact,educateyourself,betrue</t>
+  </si>
+  <si>
+    <t>facts</t>
   </si>
   <si>
     <t>https://www.instagram.com/p/BnFZRcOAo3K/?taken-by=blizzfact</t>
@@ -188,7 +272,7 @@
 #useyourbrain #factsz #goodword #truefact #youknowit #themoreyouknow #keepit100 #payattention #humbleyourself #believing #learn #liveandlearn #imjustsaying</t>
   </si>
   <si>
-    <t>themoreyouknow,humbleyourself,imjustsaying,liveandlearn,payattention,useyourbrain,keepit100,believing,youknowit,goodword,truefact,factsz,learn</t>
+    <t>themoreyouknow,humbleyourself,payattention,useyourbrain,liveandlearn,imjustsaying,keepit100,youknowit,believing,truefact,goodword,factsz,learn</t>
   </si>
   <si>
     <t>✌✌👇👆</t>
@@ -200,33 +284,18 @@
     <t>Thursday</t>
   </si>
   <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>image</t>
-  </si>
-  <si>
-    <t>blizzfact</t>
-  </si>
-  <si>
     <t>1857001571053899210</t>
   </si>
   <si>
     <t>https://scontent-mrs1-1.cdninstagram.com/vp/b57c327f0a02ae6d7517695cbf59f521/5C248C3C/t51.2885-15/e35/39371756_288356891754100_7681751821546684416_n.jpg</t>
   </si>
   <si>
-    <t>./outputs/blizzfact/images/</t>
-  </si>
-  <si>
     <t>./outputs/blizzfact/images/39371756_288356891754100_7681751821546684416_n.jpg</t>
   </si>
   <si>
     <t>39371756_288356891754100_7681751821546684416_n.jpg</t>
   </si>
   <si>
-    <t>1080x1080</t>
-  </si>
-  <si>
     <t>637.012</t>
   </si>
   <si>
@@ -239,22 +308,22 @@
     <t>NO</t>
   </si>
   <si>
-    <t>themoreyouknow,humbleyourself,imjustsaying,liveandlearn,payattention,useyourbrain,keepit100,believing,youknowit,learn</t>
+    <t>believing,learn</t>
   </si>
   <si>
     <t>factsz</t>
   </si>
   <si>
-    <t>goodword,useyourbrain</t>
+    <t>useyourbrain,goodword</t>
   </si>
   <si>
     <t>humbleyourself,believing</t>
   </si>
   <si>
-    <t>truefact,keepit100,imjustsaying,youknowit</t>
-  </si>
-  <si>
-    <t>liveandlearn,themoreyouknow,payattention</t>
+    <t>keepit100,youknowit,truefact,imjustsaying</t>
+  </si>
+  <si>
+    <t>payattention,themoreyouknow,liveandlearn</t>
   </si>
   <si>
     <t>learn</t>
@@ -271,7 +340,7 @@
 #goodword #neverforgetthat #factss #factsz #sayingsandquotes #dontthinkaboutit #factset #realness #lessonslearned</t>
   </si>
   <si>
-    <t>dontthinkaboutit,sayingsandquotes,neverforgetthat,lessonslearned,goodword,realness,factset,factss,factsz</t>
+    <t>sayingsandquotes,dontthinkaboutit,neverforgetthat,lessonslearned,realness,goodword,factset,factss,factsz</t>
   </si>
   <si>
     <t>👇✌👇</t>
@@ -313,28 +382,16 @@
     <t>273503011</t>
   </si>
   <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>dontthinkaboutit,sayingsandquotes,neverforgetthat,realness,factset,factss</t>
-  </si>
-  <si>
-    <t>factsz,factset</t>
-  </si>
-  <si>
-    <t>dontthinkaboutit,neverforgetthat</t>
+    <t>neverforgetthat</t>
+  </si>
+  <si>
+    <t>dontthinkaboutit</t>
   </si>
   <si>
     <t>factss</t>
   </si>
   <si>
-    <t>goodword</t>
-  </si>
-  <si>
     <t>sayingsandquotes</t>
-  </si>
-  <si>
-    <t>lessonslearned,realness</t>
   </si>
   <si>
     <t>https://www.instagram.com/p/BnBsvtwgbXV/?taken-by=blizzfact</t>
@@ -348,7 +405,7 @@
 #factsonfacts #realshitdoe #stilltrue #factssss #complicatedlife #goodword #interestingfacts #realshitonly #powerfull #knowledgeispower #knowledge #truths #truedat #keepitreal #lessonslearned #mindblowing #itiswhatitis #sotrue #lessonlearned #funfact #akward #positivethoughts #pretend #mindgames #quotesgram #truefact #randomness #beliveinyourself</t>
   </si>
   <si>
-    <t>interestingfacts,positivethoughts,beliveinyourself,knowledgeispower,complicatedlife,lessonslearned,lessonlearned,realshitonly,factsonfacts,itiswhatitis,realshitdoe,mindblowing,randomness,quotesgram,keepitreal,knowledge,stilltrue,powerfull,mindgames,goodword,truefact,factssss,pretend,truedat,funfact,sotrue,akward,truths</t>
+    <t>knowledgeispower,positivethoughts,beliveinyourself,interestingfacts,complicatedlife,lessonslearned,lessonlearned,factsonfacts,itiswhatitis,realshitonly,mindblowing,realshitdoe,randomness,keepitreal,quotesgram,knowledge,mindgames,stilltrue,powerfull,goodword,factssss,truefact,pretend,funfact,truedat,akward,truths,sotrue</t>
   </si>
   <si>
     <t>😛😻👇👆</t>
@@ -381,28 +438,538 @@
     <t>683630</t>
   </si>
   <si>
-    <t>interestingfacts,positivethoughts,beliveinyourself,knowledgeispower,complicatedlife,lessonlearned,realshitonly,factsonfacts,itiswhatitis,realshitdoe,mindblowing,randomness,quotesgram,keepitreal,knowledge,stilltrue,powerfull,mindgames,factssss,pretend,truedat,funfact,sotrue,akward,truths</t>
-  </si>
-  <si>
-    <t>realshitonly,complicatedlife</t>
-  </si>
-  <si>
-    <t>realshitdoe,factssss</t>
-  </si>
-  <si>
-    <t>stilltrue,factsonfacts</t>
-  </si>
-  <si>
-    <t>interestingfacts,akward,mindgames</t>
-  </si>
-  <si>
-    <t>lessonslearned,pretend,truefact,powerfull,mindblowing,beliveinyourself,truedat</t>
-  </si>
-  <si>
-    <t>randomness,lessonlearned,quotesgram,itiswhatitis,positivethoughts,knowledgeispower</t>
-  </si>
-  <si>
-    <t>knowledge,sotrue</t>
+    <t>knowledgeispower,interestingfacts,realshitonly,realshitdoe,randomness,keepitreal,mindgames,pretend</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/Bm__Tskg39J/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>Remind your friends not to sneeze 😛
+Follow: @blizzfact 👌
+👇
+TURN ON POST NOTIFICATIONS!
+👆
+#lessonslearnedinlife #quickfact #imnotanoption #tellhim #lessonlearned #itstrue #sotrue #accurate #powerfull #keepit100 #truthbetold #truthhurts #doingwork #wordoftheday #staytruetoyourself #factsoflife</t>
+  </si>
+  <si>
+    <t>lessonslearnedinlife,staytruetoyourself,lessonlearned,imnotanoption,wordoftheday,factsoflife,truthbetold,truthhurts,keepit100,powerfull,quickfact,doingwork,accurate,tellhim,itstrue,sotrue</t>
+  </si>
+  <si>
+    <t>😛👌👇👆</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/259320381/new-york-city-times-square/</t>
+  </si>
+  <si>
+    <t>Monday</t>
+  </si>
+  <si>
+    <t>1855480001957429065</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/879c329e769ac3487557c3d4e0212720/5C376E3C/t51.2885-15/e35/39665568_533795227034531_162122950860865536_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/39665568_533795227034531_162122950860865536_n.jpg</t>
+  </si>
+  <si>
+    <t>39665568_533795227034531_162122950860865536_n.jpg</t>
+  </si>
+  <si>
+    <t>387.798</t>
+  </si>
+  <si>
+    <t>New York City Times Square</t>
+  </si>
+  <si>
+    <t>259320381</t>
+  </si>
+  <si>
+    <t>lessonslearnedinlife,doingwork,itstrue</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/Bm9HhKTgc-t/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>Comment INTERESTING without getting interrupted 👇
+👇
+@blizzfact
+@blizzfact
+✌️
+#dailypositivity #quotekillahs #factsmatter #logicalthinking #factsfirst #factsthough #knowledge #funfact</t>
+  </si>
+  <si>
+    <t>dailypositivity,logicalthinking,quotekillahs,factsmatter,factsthough,factsfirst,knowledge,funfact</t>
+  </si>
+  <si>
+    <t>👇👇✌</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/330226763/liverpool-texas/</t>
+  </si>
+  <si>
+    <t>Sunday</t>
+  </si>
+  <si>
+    <t>1854671686679515053</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/d64cdd9384850ca523ac1f1d3460256a/5C31FA3D/t51.2885-15/e35/39215260_187695298683481_7539117611208933376_n.jpg,https://scontent-mrs1-1.cdninstagram.com/vp/7e9810a60a2ce0a5d2087464ef7c1ace/5C3A922E/t51.2885-15/e35/39582180_309364703158357_7037992999048970240_n.jpg,https://scontent-mrs1-1.cdninstagram.com/vp/fe88c470785ff07842b8c3509fe53f84/5C2660DD/t51.2885-15/e35/39725015_1765921670191341_3676035995813281792_n.jpg,https://scontent-mrs1-1.cdninstagram.com/vp/137e6e8a9297fd066560731871223082/5C358D4F/t51.2885-15/e35/39175642_311201446298505_4621453637346918400_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/galleries/gallery_1854671686679515053/</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/galleries/gallery_1854671686679515053/39215260_187695298683481_7539117611208933376_n.jpg,./outputs/blizzfact/galleries/gallery_1854671686679515053/39582180_309364703158357_7037992999048970240_n.jpg,./outputs/blizzfact/galleries/gallery_1854671686679515053/39725015_1765921670191341_3676035995813281792_n.jpg,./outputs/blizzfact/galleries/gallery_1854671686679515053/39175642_311201446298505_4621453637346918400_n.jpg</t>
+  </si>
+  <si>
+    <t>39215260_187695298683481_7539117611208933376_n.jpg,39582180_309364703158357_7037992999048970240_n.jpg,39725015_1765921670191341_3676035995813281792_n.jpg,39175642_311201446298505_4621453637346918400_n.jpg</t>
+  </si>
+  <si>
+    <t>619.241,401.118,282.149,799.852</t>
+  </si>
+  <si>
+    <t>Liverpool, Texas</t>
+  </si>
+  <si>
+    <t>330226763</t>
+  </si>
+  <si>
+    <t>dailypositivity,logicalthinking,quotekillahs,factsmatter,factsthough,factsfirst</t>
+  </si>
+  <si>
+    <t>factsfirst,logicalthinking,factsthough</t>
+  </si>
+  <si>
+    <t>factsmatter</t>
+  </si>
+  <si>
+    <t>quotekillahs,dailypositivity</t>
+  </si>
+  <si>
+    <t>funfact</t>
+  </si>
+  <si>
+    <t>knowledge</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/Bm8eoMAg2JV/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>Donkeys are stupid. Tag a donkey 😄
+Follow: @blizzfact for more unheard facts 😎
+👇
+TURN ON POST NOTIFICATIONS!
+👆
+#stilltrue #factssss #imnotanoption #knowyourself #inspirationalwords #truefact #staytruetoyourself #humbleyourself #trueshit #educateyourself #thinkpositive</t>
+  </si>
+  <si>
+    <t>inspirationalwords,staytruetoyourself,educateyourself,humbleyourself,imnotanoption,thinkpositive,knowyourself,stilltrue,truefact,trueshit,factssss</t>
+  </si>
+  <si>
+    <t>😄😎👇👆</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/213281320/dubai-united-arab-emirates/</t>
+  </si>
+  <si>
+    <t>1854491849637716565</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/96e049fead00977e2dcd29e072588177/5C35F30F/t51.2885-15/e35/39486023_246451566071439_8969095133819568128_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/39486023_246451566071439_8969095133819568128_n.jpg</t>
+  </si>
+  <si>
+    <t>39486023_246451566071439_8969095133819568128_n.jpg</t>
+  </si>
+  <si>
+    <t>343.371</t>
+  </si>
+  <si>
+    <t>Dubai, United Arab Emirates</t>
+  </si>
+  <si>
+    <t>213281320</t>
+  </si>
+  <si>
+    <t>knowyourself,trueshit</t>
+  </si>
+  <si>
+    <t>imnotanoption</t>
+  </si>
+  <si>
+    <t>factssss</t>
+  </si>
+  <si>
+    <t>stilltrue</t>
+  </si>
+  <si>
+    <t>staytruetoyourself,humbleyourself</t>
+  </si>
+  <si>
+    <t>inspirationalwords,truefact,knowyourself</t>
+  </si>
+  <si>
+    <t>educateyourself,trueshit,thinkpositive</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/Bm6MKGqgKXH/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>I drink maybe hundreds ✌️
+Follow: @blizzfact 😎👇
+👇
+TURN ON POST NOTIFICATIONS!
+👆
+#factset #amazingfacts #factssss #interestingfact #goodword #worldfacts #complicatedlife #ridiculous #philosopher #tootrue #lifelesson #inspirationalwords #themoreyouknow #thinkpositive #factsoflife #secrets #positivemind #educateyourself #knowledgeofself #realshittho #facts💯 #truthbetold #lessonlearned #realtalk #forrealtho #humbleyourself</t>
+  </si>
+  <si>
+    <t>inspirationalwords,interestingfact,complicatedlife,educateyourself,knowledgeofself,themoreyouknow,humbleyourself,lessonlearned,thinkpositive,amazingfacts,positivemind,factsoflife,philosopher,realshittho,truthbetold,lifelesson,worldfacts,ridiculous,forrealtho,realtalk,goodword,factssss,secrets,factset,tootrue,facts💯</t>
+  </si>
+  <si>
+    <t>✌😎👇👇👆💯</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/375269519489153/paris/</t>
+  </si>
+  <si>
+    <t>Saturday</t>
+  </si>
+  <si>
+    <t>1853847667524806087</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/4a5d024463ef7dbe64358d89557fe091/5C328AE3/t51.2885-15/e35/37508014_272713573342956_6926970173211541504_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/37508014_272713573342956_6926970173211541504_n.jpg</t>
+  </si>
+  <si>
+    <t>37508014_272713573342956_6926970173211541504_n.jpg</t>
+  </si>
+  <si>
+    <t>629.882</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>375269519489153</t>
+  </si>
+  <si>
+    <t>interestingfact,knowledgeofself,philosopher,realshittho,worldfacts,ridiculous,forrealtho,realtalk,secrets,tootrue,facts💯</t>
+  </si>
+  <si>
+    <t>complicatedlife,factset</t>
+  </si>
+  <si>
+    <t>interestingfact,factssss</t>
+  </si>
+  <si>
+    <t>amazingfacts,worldfacts</t>
+  </si>
+  <si>
+    <t>goodword</t>
+  </si>
+  <si>
+    <t>humbleyourself,realshittho</t>
+  </si>
+  <si>
+    <t>philosopher</t>
+  </si>
+  <si>
+    <t>facts💯,lessonlearned,lifelesson,thinkpositive,themoreyouknow,secrets,positivemind,ridiculous,educateyourself,knowledgeofself</t>
+  </si>
+  <si>
+    <t>realtalk</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/Bm4UdTegtoi/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>I want to adapt coyote ✌️
+Follow: @blizzfact 😻
+👇
+TURN ON POST NOTIFICATIONS!
+👆
+#factsallday #thoughs #useyourbrain #factsonfacts #superherofacts #amazingfacts #dontthinkaboutit #phylosophy #nobullshit #youwouldntunderstand #wordsoftheday #payattention #sadbuttrue #mindblowing #understand #lessonslearned #justbeinghonest #imjustsaying #truthhurts #truthseeker #whatthehell #goodthoughts #truthbetold #realness #thinkpositive #questioneverything #inspirationalwords #lessonlearned</t>
+  </si>
+  <si>
+    <t>youwouldntunderstand,questioneverything,inspirationalwords,dontthinkaboutit,justbeinghonest,superherofacts,lessonslearned,lessonlearned,thinkpositive,wordsoftheday,factsonfacts,amazingfacts,goodthoughts,useyourbrain,imjustsaying,payattention,whatthehell,mindblowing,factsallday,truthseeker,truthbetold,nobullshit,understand,truthhurts,phylosophy,sadbuttrue,realness,thoughs</t>
+  </si>
+  <si>
+    <t>✌😻👇👆</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/212923417/disneys-hollywood-studios/</t>
+  </si>
+  <si>
+    <t>1853321221370993186</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/12bfef1edf7e66913214b945640d56f9/5C2BEF5F/t51.2885-15/e35/39306074_2125296627731245_2603488370290065408_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/39306074_2125296627731245_2603488370290065408_n.jpg</t>
+  </si>
+  <si>
+    <t>39306074_2125296627731245_2603488370290065408_n.jpg</t>
+  </si>
+  <si>
+    <t>609.329</t>
+  </si>
+  <si>
+    <t>Disney's Hollywood Studios</t>
+  </si>
+  <si>
+    <t>212923417</t>
+  </si>
+  <si>
+    <t>youwouldntunderstand,questioneverything,justbeinghonest,superherofacts,goodthoughts,whatthehell,factsallday,nobullshit,phylosophy,sadbuttrue,thoughs</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/p/Bm1sVjcAGbf/?taken-by=blizzfact</t>
+  </si>
+  <si>
+    <t>Comment your city you are in 👍
+Follow: @blizzfact ✌
+👇
+TURN ON POST NOTIFICATIONS!
+👆
+#sayingsandquotes #amazingfacts #whenitsreal #quickfact #factsss #factss #factsb #educateyourself #liveandlearn #positivethoughts #inspirationalwords #lifelesson #wordsoftheday #accurate #quotesgram #youknowit #mindblowing #truthseeker #betrue #factsonly #positivemind #humbleyourself #funnybuttrue #truuu #understand</t>
+  </si>
+  <si>
+    <t>inspirationalwords,sayingsandquotes,positivethoughts,educateyourself,humbleyourself,wordsoftheday,funnybuttrue,amazingfacts,positivemind,liveandlearn,mindblowing,whenitsreal,truthseeker,lifelesson,understand,quotesgram,factsonly,youknowit,quickfact,accurate,factsss,factsb,factss,betrue,truuu</t>
+  </si>
+  <si>
+    <t>👍✌👇👆</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/explore/locations/127958949/caesars-palace/</t>
+  </si>
+  <si>
+    <t>1852581816939079391</t>
+  </si>
+  <si>
+    <t>https://scontent-mrs1-1.cdninstagram.com/vp/0fccad5b4280d3dd4e1f0610aa53408c/5C3114D8/t51.2885-15/e35/39361456_1151656778315071_3500535798078373888_n.jpg</t>
+  </si>
+  <si>
+    <t>./outputs/blizzfact/images/39361456_1151656778315071_3500535798078373888_n.jpg</t>
+  </si>
+  <si>
+    <t>39361456_1151656778315071_3500535798078373888_n.jpg</t>
+  </si>
+  <si>
+    <t>581.975</t>
+  </si>
+  <si>
+    <t>Caesars Palace</t>
+  </si>
+  <si>
+    <t>127958949</t>
+  </si>
+  <si>
+    <t>factsonly,factsss,truuu</t>
+  </si>
+  <si>
+    <t>GENERAL ANALYSIS OF THE ACCOUNT</t>
+  </si>
+  <si>
+    <t>Average size of the media (image or video) (in KB)</t>
+  </si>
+  <si>
+    <t>Average amount of posts per day (24-hour period)</t>
+  </si>
+  <si>
+    <t>Day of the week account posting the most of the content</t>
+  </si>
+  <si>
+    <t>Percentage of video content</t>
+  </si>
+  <si>
+    <t>Percentage of image content</t>
+  </si>
+  <si>
+    <t>Percentage of gallery content</t>
+  </si>
+  <si>
+    <t>Average amount of words being used in the caption (eliminating hashtags and emoji's)</t>
+  </si>
+  <si>
+    <t>Amount of unique words being used on all captions</t>
+  </si>
+  <si>
+    <t>Average amount of hashtags being used in the caption</t>
+  </si>
+  <si>
+    <t>List of repetitive hashtags used in captions (mostly used)</t>
+  </si>
+  <si>
+    <t>List of repetitive hashtags used in captions (mostly used) (spin syntax format)</t>
+  </si>
+  <si>
+    <t>List of unique hashtags used in captions</t>
+  </si>
+  <si>
+    <t>List of unique hashtags used in captions (spin syntax format)</t>
+  </si>
+  <si>
+    <t>Hashtag Uniqueness in the captions</t>
+  </si>
+  <si>
+    <t>Average percentage rate of the same hashtags being used on every caption</t>
+  </si>
+  <si>
+    <t>How many hashtags account got featured under any of the TOP 9 posts (all unique hashtags / got featured)?</t>
+  </si>
+  <si>
+    <t>Which category of hashtags account used the most in the captions?</t>
+  </si>
+  <si>
+    <t>Average percentage rate of the same words being used on every caption</t>
+  </si>
+  <si>
+    <t>Average amount of emojis being used in the captions</t>
+  </si>
+  <si>
+    <t>Spintax of all emojis being used</t>
+  </si>
+  <si>
+    <t>Average amount of tagged accounts on the post</t>
+  </si>
+  <si>
+    <t>Average amount of mentioned accounts in the caption</t>
+  </si>
+  <si>
+    <t>Average amount of likes of the post</t>
+  </si>
+  <si>
+    <t>Average amount of comments of the post</t>
+  </si>
+  <si>
+    <t>Average percentage rate of GHOST LIKERS (the higher percentage rate shows how likely account has fake followers or uses engagement pods/like rounds)</t>
+  </si>
+  <si>
+    <t>Average percentage rate of GHOST COMMENTERS (the higher percentage rate shows how likely account has fake comments or either uses automated comment pods</t>
+  </si>
+  <si>
+    <t>Average engagement rate of the post</t>
+  </si>
+  <si>
+    <t>Average amount of locations tagged on the post (can't be higher than 1; 1 means that all posts had their locations tagged)</t>
+  </si>
+  <si>
+    <t>How many times did account got featured on any of TOP 9 posts under any of the used tagged locations?</t>
+  </si>
+  <si>
+    <t>Predictive account age (only if you chose to scrape all account posts) or for how long account has been posting</t>
+  </si>
+  <si>
+    <t>List of 0k-10k hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 10k-20k hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 20k-50k hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 50k-100k hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 100k-200k hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 200k-500k hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 500k-2M hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 2M-5M hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of 5M-999M hashtags (duplicates removed)</t>
+  </si>
+  <si>
+    <t>Caption uniqueness (OVERALL)</t>
+  </si>
+  <si>
+    <t>Hashtag uniqueness</t>
+  </si>
+  <si>
+    <t>Dictionary uniqueness</t>
+  </si>
+  <si>
+    <t>Amount of different emojis</t>
+  </si>
+  <si>
+    <t>List of all emojis used (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of tagged accounts (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of mentioned accounts (duplicates removed)</t>
+  </si>
+  <si>
+    <t>List of tagged locations' URLs (duplicates removed)</t>
+  </si>
+  <si>
+    <t>522.613</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>18.8</t>
+  </si>
+  <si>
+    <t>funnybuttrue,tellhim,lessonlearned,factsb,knowledge,lifelesson,factsonfacts,stilltrue,mindblowing,thinkpositive,amazingfacts,akward,accurate,sayingsandquotes,themoreyouknow,whenitsreal,dontthinkaboutit,complicatedlife,truths,useyourbrain,factsz,sotrue,goodword,positivemind,imjustsaying,understand,positivethoughts,beliveinyourself,wordoftheday,wordsoftheday,quotesgram,factss,factsoflife,payattention,keepit100,truthhurts,inspirationalwords,staytruetoyourself,itiswhatitis,realness,humbleyourself,youknowit,powerfull,liveandlearn,funfact,lessonslearned,imnotanoption,quickfact,truthseeker,factssss,truedat,educateyourself,betrue,truefact,factset,truthbetold</t>
+  </si>
+  <si>
+    <t>{funnybuttrue|tellhim|lessonlearned|factsb|knowledge|lifelesson|factsonfacts|stilltrue|mindblowing|thinkpositive|amazingfacts|akward|accurate|sayingsandquotes|themoreyouknow|whenitsreal|dontthinkaboutit|complicatedlife|truths|useyourbrain|factsz|sotrue|goodword|positivemind|imjustsaying|understand|positivethoughts|beliveinyourself|wordoftheday|wordsoftheday|quotesgram|factss|factsoflife|payattention|keepit100|truthhurts|inspirationalwords|staytruetoyourself|itiswhatitis|realness|humbleyourself|youknowit|powerfull|liveandlearn|funfact|lessonslearned|imnotanoption|quickfact|truthseeker|factssss|truedat|educateyourself|betrue|truefact|factset|truthbetold}</t>
+  </si>
+  <si>
+    <t>facts💯,itstrue,pretend,facts,justbeinghonest,mindgames,forrealtho,whatthehell,trueshit,knowyourself,randomness,factsthough,nobullshit,factsonly,keepitreal,questioneverything,interestingfact,realtalk,goodthoughts,youwouldntunderstand,neverforgetthat,dailypositivity,factsss,factsfirst,knowledgeispower,secrets,lessonslearnedinlife,factsmatter,lifeslessons,superherofacts,worldfacts,factsallday,ridiculous,philosopher,phylosophy,thoughs,truuu,logicalthinking,believing,realtalktho,doingwork,realshitonly,wikipedia,learn,realshitdoe,knowledgeofself,quotekillahs,realshittho,sadbuttrue,tootrue,interestingfacts,questionmark</t>
+  </si>
+  <si>
+    <t>{facts💯|itstrue|pretend|facts|justbeinghonest|mindgames|forrealtho|whatthehell|trueshit|knowyourself|randomness|factsthough|nobullshit|factsonly|keepitreal|questioneverything|interestingfact|realtalk|goodthoughts|youwouldntunderstand|neverforgetthat|dailypositivity|factsss|factsfirst|knowledgeispower|secrets|lessonslearnedinlife|factsmatter|lifeslessons|superherofacts|worldfacts|factsallday|ridiculous|philosopher|phylosophy|thoughs|truuu|logicalthinking|believing|realtalktho|doingwork|realshitonly|wikipedia|learn|realshitdoe|knowledgeofself|quotekillahs|realshittho|sadbuttrue|tootrue|interestingfacts|questionmark}</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>{😎|👌|😄|✌|😻|👆|💯|👇|😛|👍}</t>
+  </si>
+  <si>
+    <t>😎,👌,😄,✌,😻,👆,💯,👇,😛,👍</t>
+  </si>
+  <si>
+    <t>factsz,factsfirst,logicalthinking,factsthough,imnotanoption,complicatedlife,factset</t>
+  </si>
+  <si>
+    <t>tellhim,factsb,whenitsreal,dontthinkaboutit,factsmatter,factssss,interestingfact,factssss</t>
+  </si>
+  <si>
+    <t>factss,quotekillahs,dailypositivity,stilltrue,amazingfacts,worldfacts</t>
+  </si>
+  <si>
+    <t>lifeslessons,realtalktho,useyourbrain,goodword,goodword</t>
+  </si>
+  <si>
+    <t>funnybuttrue,akward,sayingsandquotes,wikipedia,questionmark,humbleyourself,believing,sayingsandquotes,staytruetoyourself,humbleyourself,humbleyourself,realshittho</t>
+  </si>
+  <si>
+    <t>truths,imjustsaying,beliveinyourself,factsoflife,realness,truedat,keepit100,youknowit,truefact,imjustsaying,inspirationalwords,truefact,knowyourself,philosopher</t>
+  </si>
+  <si>
+    <t>positivemind,wordoftheday,itiswhatitis,liveandlearn,funfact,educateyourself,betrue,payattention,themoreyouknow,liveandlearn,funfact,educateyourself,trueshit,thinkpositive,facts💯,lessonlearned,lifelesson,thinkpositive,themoreyouknow,secrets,positivemind,ridiculous,educateyourself,knowledgeofself</t>
+  </si>
+  <si>
+    <t>facts,learn,knowledge,realtalk</t>
   </si>
 </sst>
 </file>
@@ -914,7 +1481,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:BY4"/>
+  <dimension ref="A1:BY11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1128,14 +1695,14 @@
         <v>68</v>
       </c>
       <c r="I2" s="17">
-        <v>970</v>
+        <v>1207</v>
       </c>
       <c r="J2" s="17"/>
       <c r="K2" s="17">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="L2" s="18">
-        <v>0.07863906275076232</v>
+        <v>0.1015931470658874</v>
       </c>
       <c r="M2" s="17"/>
       <c r="N2" s="17">
@@ -1151,38 +1718,38 @@
         <v>57</v>
       </c>
       <c r="R2" s="19">
-        <v>43342</v>
+        <v>43343</v>
       </c>
       <c r="S2" s="17" t="s">
         <v>55</v>
       </c>
       <c r="T2" s="17">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="U2" s="17" t="s">
         <v>72</v>
       </c>
       <c r="V2" s="17">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="W2" s="18">
-        <v>0.7692307692307693</v>
-      </c>
-      <c r="X2" s="17" t="s">
+        <v>0.2083333333333333</v>
+      </c>
+      <c r="X2" s="17"/>
+      <c r="Y2" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="Y2" s="17">
-        <v>1</v>
-      </c>
-      <c r="Z2" s="18">
-        <v>0.07692307692307693</v>
-      </c>
-      <c r="AA2" s="17"/>
       <c r="AB2" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AC2" s="18">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="AD2" s="17"/>
       <c r="AE2" s="17">
@@ -1198,34 +1765,34 @@
         <v>2</v>
       </c>
       <c r="AI2" s="18">
-        <v>0.1538461538461539</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="AJ2" s="17" t="s">
         <v>75</v>
       </c>
       <c r="AK2" s="17">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AL2" s="18">
-        <v>0.1538461538461539</v>
+        <v>0.2083333333333333</v>
       </c>
       <c r="AM2" s="17" t="s">
         <v>76</v>
       </c>
       <c r="AN2" s="17">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AO2" s="18">
-        <v>0.3076923076923077</v>
+        <v>0.25</v>
       </c>
       <c r="AP2" s="17" t="s">
         <v>77</v>
       </c>
       <c r="AQ2" s="17">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="AR2" s="18">
-        <v>0.2307692307692308</v>
+        <v>0.2916666666666667</v>
       </c>
       <c r="AS2" s="17"/>
       <c r="AT2" s="17">
@@ -1241,19 +1808,19 @@
         <v>1</v>
       </c>
       <c r="AX2" s="18">
-        <v>0.07692307692307693</v>
+        <v>0.04166666666666666</v>
       </c>
       <c r="AY2" s="17">
         <v>2</v>
       </c>
       <c r="AZ2" s="17">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="BA2" s="18">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="BB2" s="18">
-        <v>0.4166666666666667</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="BU2" s="17" t="s">
         <v>57</v>
@@ -1267,42 +1834,44 @@
       <c r="BX2" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="BY2" s="17"/>
+      <c r="BY2" s="17">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:77" ht="40" customHeight="1">
       <c r="A3" s="17" t="s">
         <v>79</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="D3" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="F3" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="F3" s="17" t="s">
-        <v>90</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="17" t="s">
-        <v>92</v>
-      </c>
       <c r="I3" s="17">
-        <v>615</v>
+        <v>1184</v>
       </c>
       <c r="J3" s="17"/>
       <c r="K3" s="17">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L3" s="18">
-        <v>0.04951051195634729</v>
+        <v>0.09558882395324633</v>
       </c>
       <c r="M3" s="17"/>
       <c r="N3" s="17">
@@ -1318,83 +1887,81 @@
         <v>83</v>
       </c>
       <c r="R3" s="19">
-        <v>43341</v>
+        <v>43342</v>
       </c>
       <c r="S3" s="17" t="s">
         <v>81</v>
       </c>
       <c r="T3" s="17">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="U3" s="17" t="s">
+        <v>93</v>
+      </c>
+      <c r="V3" s="17">
+        <v>2</v>
+      </c>
+      <c r="W3" s="18">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="X3" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z3" s="18">
+        <v>0.07692307692307693</v>
+      </c>
+      <c r="AA3" s="17"/>
+      <c r="AB3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="17"/>
+      <c r="AE3" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="AH3" s="17">
+        <v>2</v>
+      </c>
+      <c r="AI3" s="18">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="AJ3" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="V3" s="17">
-        <v>6</v>
-      </c>
-      <c r="W3" s="18">
-        <v>0.6666666666666666</v>
-      </c>
-      <c r="X3" s="17" t="s">
+      <c r="AK3" s="17">
+        <v>2</v>
+      </c>
+      <c r="AL3" s="18">
+        <v>0.1538461538461539</v>
+      </c>
+      <c r="AM3" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="Y3" s="17">
-        <v>2</v>
-      </c>
-      <c r="Z3" s="18">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="AA3" s="17" t="s">
+      <c r="AN3" s="17">
+        <v>4</v>
+      </c>
+      <c r="AO3" s="18">
+        <v>0.3076923076923077</v>
+      </c>
+      <c r="AP3" s="17" t="s">
         <v>98</v>
       </c>
-      <c r="AB3" s="17">
-        <v>2</v>
-      </c>
-      <c r="AC3" s="18">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="AD3" s="17" t="s">
-        <v>99</v>
-      </c>
-      <c r="AE3" s="17">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="18">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="AG3" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH3" s="17">
-        <v>1</v>
-      </c>
-      <c r="AI3" s="18">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="AJ3" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="AK3" s="17">
-        <v>1</v>
-      </c>
-      <c r="AL3" s="18">
-        <v>0.1111111111111111</v>
-      </c>
-      <c r="AM3" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="AN3" s="17">
-        <v>2</v>
-      </c>
-      <c r="AO3" s="18">
-        <v>0.2222222222222222</v>
-      </c>
-      <c r="AP3" s="17"/>
       <c r="AQ3" s="17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AR3" s="18">
-        <v>0</v>
+        <v>0.2307692307692308</v>
       </c>
       <c r="AS3" s="17"/>
       <c r="AT3" s="17">
@@ -1403,75 +1970,75 @@
       <c r="AU3" s="18">
         <v>0</v>
       </c>
-      <c r="AV3" s="17"/>
+      <c r="AV3" s="17" t="s">
+        <v>99</v>
+      </c>
       <c r="AW3" s="17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX3" s="18">
-        <v>0</v>
+        <v>0.07692307692307693</v>
       </c>
       <c r="AY3" s="17">
         <v>2</v>
       </c>
       <c r="AZ3" s="17">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="BA3" s="18">
         <v>0</v>
       </c>
       <c r="BB3" s="18">
-        <v>1</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="BU3" s="17" t="s">
         <v>83</v>
       </c>
       <c r="BV3" s="17" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="BW3" s="17" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="BX3" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="BY3" s="17">
-        <v>1</v>
-      </c>
+        <v>92</v>
+      </c>
+      <c r="BY3" s="17"/>
     </row>
     <row r="4" spans="1:77" ht="40" customHeight="1">
       <c r="A4" s="17" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" s="17" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" s="17" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="E4" s="17" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="E4" s="17" t="s">
+      <c r="F4" s="17" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>112</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>67</v>
       </c>
       <c r="H4" s="17" t="s">
         <v>113</v>
       </c>
       <c r="I4" s="17">
-        <v>767</v>
+        <v>725</v>
       </c>
       <c r="J4" s="17"/>
       <c r="K4" s="17">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L4" s="18">
-        <v>0.06154710319370887</v>
+        <v>0.05820190537186774</v>
       </c>
       <c r="M4" s="17"/>
       <c r="N4" s="17">
@@ -1484,88 +2051,80 @@
         <v>1</v>
       </c>
       <c r="Q4" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="R4" s="19">
-        <v>43340</v>
+        <v>43341</v>
       </c>
       <c r="S4" s="17" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="T4" s="17">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="U4" s="17" t="s">
         <v>116</v>
       </c>
       <c r="V4" s="17">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="W4" s="18">
-        <v>0.8928571428571429</v>
-      </c>
-      <c r="X4" s="17" t="s">
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="X4" s="17"/>
+      <c r="Y4" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="Y4" s="17">
-        <v>2</v>
-      </c>
-      <c r="Z4" s="18">
-        <v>0.08</v>
-      </c>
-      <c r="AA4" s="17" t="s">
+      <c r="AB4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="18">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="AD4" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="AB4" s="17">
-        <v>2</v>
-      </c>
-      <c r="AC4" s="18">
-        <v>0.08</v>
-      </c>
-      <c r="AD4" s="17" t="s">
+      <c r="AE4" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="18">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="AG4" s="17"/>
+      <c r="AH4" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="AE4" s="17">
-        <v>2</v>
-      </c>
-      <c r="AF4" s="18">
-        <v>0.08</v>
-      </c>
-      <c r="AG4" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="AH4" s="17">
+      <c r="AK4" s="17">
         <v>1</v>
       </c>
-      <c r="AI4" s="18">
-        <v>0.04</v>
-      </c>
-      <c r="AJ4" s="17" t="s">
-        <v>120</v>
-      </c>
-      <c r="AK4" s="17">
-        <v>3</v>
-      </c>
       <c r="AL4" s="18">
-        <v>0.12</v>
-      </c>
-      <c r="AM4" s="17" t="s">
-        <v>121</v>
-      </c>
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="AM4" s="17"/>
       <c r="AN4" s="17">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="AO4" s="18">
-        <v>0.28</v>
-      </c>
-      <c r="AP4" s="17" t="s">
-        <v>122</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="AP4" s="17"/>
       <c r="AQ4" s="17">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AR4" s="18">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="AS4" s="17"/>
       <c r="AT4" s="17">
@@ -1574,23 +2133,27 @@
       <c r="AU4" s="18">
         <v>0</v>
       </c>
-      <c r="AV4" s="17" t="s">
-        <v>123</v>
-      </c>
+      <c r="AV4" s="17"/>
       <c r="AW4" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="18">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="17">
         <v>2</v>
       </c>
-      <c r="AX4" s="18">
-        <v>0.08</v>
-      </c>
-      <c r="AY4" s="17"/>
-      <c r="AZ4" s="17"/>
-      <c r="BA4" s="18"/>
+      <c r="AZ4" s="17">
+        <v>5</v>
+      </c>
+      <c r="BA4" s="18">
+        <v>0</v>
+      </c>
       <c r="BB4" s="18">
-        <v>0.5833333333333334</v>
+        <v>0.2</v>
       </c>
       <c r="BU4" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="BV4" s="17" t="s">
         <v>114</v>
@@ -1601,7 +2164,1456 @@
       <c r="BX4" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="BY4" s="17"/>
+      <c r="BY4" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:77" ht="40" customHeight="1">
+      <c r="A5" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E5" s="17" t="s">
+        <v>128</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="G5" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I5" s="17">
+        <v>816</v>
+      </c>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17">
+        <v>0</v>
+      </c>
+      <c r="L5" s="18">
+        <v>0.06532703546553519</v>
+      </c>
+      <c r="M5" s="17"/>
+      <c r="N5" s="17">
+        <v>0</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P5" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="R5" s="19">
+        <v>43340</v>
+      </c>
+      <c r="S5" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="T5" s="17">
+        <v>28</v>
+      </c>
+      <c r="U5" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="V5" s="17">
+        <v>8</v>
+      </c>
+      <c r="W5" s="18">
+        <v>0.2857142857142857</v>
+      </c>
+      <c r="X5" s="17"/>
+      <c r="Y5" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="17"/>
+      <c r="AB5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="17"/>
+      <c r="AE5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="17"/>
+      <c r="AH5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="17"/>
+      <c r="AK5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM5" s="17"/>
+      <c r="AN5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="17"/>
+      <c r="AQ5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="17"/>
+      <c r="AT5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="17"/>
+      <c r="AW5" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="18">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="17">
+        <v>3</v>
+      </c>
+      <c r="AZ5" s="17">
+        <v>7</v>
+      </c>
+      <c r="BA5" s="18">
+        <v>0.4166666666666667</v>
+      </c>
+      <c r="BB5" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="BU5" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="BV5" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="BW5" s="17" t="s">
+        <v>132</v>
+      </c>
+      <c r="BX5" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY5" s="17"/>
+    </row>
+    <row r="6" spans="1:77" ht="40" customHeight="1">
+      <c r="A6" s="17" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>140</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>141</v>
+      </c>
+      <c r="D6" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>142</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>143</v>
+      </c>
+      <c r="G6" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" s="17" t="s">
+        <v>144</v>
+      </c>
+      <c r="I6" s="17">
+        <v>797</v>
+      </c>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17">
+        <v>6</v>
+      </c>
+      <c r="L6" s="18">
+        <v>0.06428628612601073</v>
+      </c>
+      <c r="M6" s="17"/>
+      <c r="N6" s="17">
+        <v>0</v>
+      </c>
+      <c r="O6" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P6" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="R6" s="19">
+        <v>43339</v>
+      </c>
+      <c r="S6" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="T6" s="17">
+        <v>16</v>
+      </c>
+      <c r="U6" s="17" t="s">
+        <v>147</v>
+      </c>
+      <c r="V6" s="17">
+        <v>3</v>
+      </c>
+      <c r="W6" s="18">
+        <v>0.1875</v>
+      </c>
+      <c r="X6" s="17"/>
+      <c r="Y6" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="17"/>
+      <c r="AE6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="17"/>
+      <c r="AH6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="17"/>
+      <c r="AK6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="17"/>
+      <c r="AN6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP6" s="17"/>
+      <c r="AQ6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS6" s="17"/>
+      <c r="AT6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV6" s="17"/>
+      <c r="AW6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="18">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="17">
+        <v>11</v>
+      </c>
+      <c r="BA6" s="18">
+        <v>0</v>
+      </c>
+      <c r="BB6" s="18">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="BU6" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="BV6" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="BW6" s="17" t="s">
+        <v>146</v>
+      </c>
+      <c r="BX6" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY6" s="17"/>
+    </row>
+    <row r="7" spans="1:77" ht="40" customHeight="1">
+      <c r="A7" s="17" t="s">
+        <v>148</v>
+      </c>
+      <c r="B7" s="17" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="17" t="s">
+        <v>155</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>156</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>157</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>158</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="H7" s="17" t="s">
+        <v>159</v>
+      </c>
+      <c r="I7" s="17">
+        <v>1065</v>
+      </c>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17">
+        <v>6</v>
+      </c>
+      <c r="L7" s="18">
+        <v>0.08574173404851493</v>
+      </c>
+      <c r="M7" s="17"/>
+      <c r="N7" s="17">
+        <v>0</v>
+      </c>
+      <c r="O7" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="R7" s="19">
+        <v>43338</v>
+      </c>
+      <c r="S7" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="T7" s="17">
+        <v>8</v>
+      </c>
+      <c r="U7" s="17" t="s">
+        <v>162</v>
+      </c>
+      <c r="V7" s="17">
+        <v>6</v>
+      </c>
+      <c r="W7" s="18">
+        <v>0.75</v>
+      </c>
+      <c r="X7" s="17" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y7" s="17">
+        <v>3</v>
+      </c>
+      <c r="Z7" s="18">
+        <v>0.375</v>
+      </c>
+      <c r="AA7" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="AB7" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC7" s="18">
+        <v>0.125</v>
+      </c>
+      <c r="AD7" s="17" t="s">
+        <v>165</v>
+      </c>
+      <c r="AE7" s="17">
+        <v>2</v>
+      </c>
+      <c r="AF7" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="AG7" s="17"/>
+      <c r="AH7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="17"/>
+      <c r="AK7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="17"/>
+      <c r="AN7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="17" t="s">
+        <v>166</v>
+      </c>
+      <c r="AQ7" s="17">
+        <v>1</v>
+      </c>
+      <c r="AR7" s="18">
+        <v>0.125</v>
+      </c>
+      <c r="AS7" s="17"/>
+      <c r="AT7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="17" t="s">
+        <v>167</v>
+      </c>
+      <c r="AW7" s="17">
+        <v>1</v>
+      </c>
+      <c r="AX7" s="18">
+        <v>0.125</v>
+      </c>
+      <c r="AY7" s="17">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="17">
+        <v>5</v>
+      </c>
+      <c r="BA7" s="18">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="18">
+        <v>0.2</v>
+      </c>
+      <c r="BU7" s="17" t="s">
+        <v>152</v>
+      </c>
+      <c r="BV7" s="17" t="s">
+        <v>160</v>
+      </c>
+      <c r="BW7" s="17" t="s">
+        <v>161</v>
+      </c>
+      <c r="BX7" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="BY7" s="17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:77" ht="40" customHeight="1">
+      <c r="A8" s="17" t="s">
+        <v>168</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>176</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>177</v>
+      </c>
+      <c r="I8" s="17">
+        <v>1402</v>
+      </c>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17">
+        <v>9</v>
+      </c>
+      <c r="L8" s="18">
+        <v>0.1129613321591546</v>
+      </c>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17">
+        <v>0</v>
+      </c>
+      <c r="O8" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P8" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="R8" s="19">
+        <v>43338</v>
+      </c>
+      <c r="S8" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="T8" s="17">
+        <v>11</v>
+      </c>
+      <c r="U8" s="17" t="s">
+        <v>180</v>
+      </c>
+      <c r="V8" s="17">
+        <v>2</v>
+      </c>
+      <c r="W8" s="18">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="X8" s="17" t="s">
+        <v>181</v>
+      </c>
+      <c r="Y8" s="17">
+        <v>1</v>
+      </c>
+      <c r="Z8" s="18">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="AA8" s="17" t="s">
+        <v>182</v>
+      </c>
+      <c r="AB8" s="17">
+        <v>1</v>
+      </c>
+      <c r="AC8" s="18">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="AD8" s="17" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE8" s="17">
+        <v>1</v>
+      </c>
+      <c r="AF8" s="18">
+        <v>0.09090909090909091</v>
+      </c>
+      <c r="AG8" s="17"/>
+      <c r="AH8" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="17" t="s">
+        <v>184</v>
+      </c>
+      <c r="AK8" s="17">
+        <v>2</v>
+      </c>
+      <c r="AL8" s="18">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="AM8" s="17" t="s">
+        <v>185</v>
+      </c>
+      <c r="AN8" s="17">
+        <v>3</v>
+      </c>
+      <c r="AO8" s="18">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="AP8" s="17" t="s">
+        <v>186</v>
+      </c>
+      <c r="AQ8" s="17">
+        <v>3</v>
+      </c>
+      <c r="AR8" s="18">
+        <v>0.2727272727272727</v>
+      </c>
+      <c r="AS8" s="17"/>
+      <c r="AT8" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="17"/>
+      <c r="AW8" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="18">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="17">
+        <v>5</v>
+      </c>
+      <c r="AZ8" s="17">
+        <v>10</v>
+      </c>
+      <c r="BA8" s="18">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="BB8" s="18">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="BU8" s="17" t="s">
+        <v>172</v>
+      </c>
+      <c r="BV8" s="17" t="s">
+        <v>178</v>
+      </c>
+      <c r="BW8" s="17" t="s">
+        <v>179</v>
+      </c>
+      <c r="BX8" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY8" s="17"/>
+    </row>
+    <row r="9" spans="1:77" ht="40" customHeight="1">
+      <c r="A9" s="17" t="s">
+        <v>187</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="I9" s="17">
+        <v>1267</v>
+      </c>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17">
+        <v>3</v>
+      </c>
+      <c r="L9" s="18">
+        <v>0.1016732047073893</v>
+      </c>
+      <c r="M9" s="17"/>
+      <c r="N9" s="17">
+        <v>0</v>
+      </c>
+      <c r="O9" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P9" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="R9" s="19">
+        <v>43337</v>
+      </c>
+      <c r="S9" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="T9" s="17">
+        <v>26</v>
+      </c>
+      <c r="U9" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="V9" s="17">
+        <v>11</v>
+      </c>
+      <c r="W9" s="18">
+        <v>0.4230769230769231</v>
+      </c>
+      <c r="X9" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y9" s="17">
+        <v>2</v>
+      </c>
+      <c r="Z9" s="18">
+        <v>0.09523809523809523</v>
+      </c>
+      <c r="AA9" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB9" s="17">
+        <v>2</v>
+      </c>
+      <c r="AC9" s="18">
+        <v>0.09523809523809523</v>
+      </c>
+      <c r="AD9" s="17" t="s">
+        <v>203</v>
+      </c>
+      <c r="AE9" s="17">
+        <v>2</v>
+      </c>
+      <c r="AF9" s="18">
+        <v>0.09523809523809523</v>
+      </c>
+      <c r="AG9" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="AH9" s="17">
+        <v>1</v>
+      </c>
+      <c r="AI9" s="18">
+        <v>0.04761904761904762</v>
+      </c>
+      <c r="AJ9" s="17" t="s">
+        <v>205</v>
+      </c>
+      <c r="AK9" s="17">
+        <v>2</v>
+      </c>
+      <c r="AL9" s="18">
+        <v>0.09523809523809523</v>
+      </c>
+      <c r="AM9" s="17" t="s">
+        <v>206</v>
+      </c>
+      <c r="AN9" s="17">
+        <v>1</v>
+      </c>
+      <c r="AO9" s="18">
+        <v>0.04761904761904762</v>
+      </c>
+      <c r="AP9" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="AQ9" s="17">
+        <v>10</v>
+      </c>
+      <c r="AR9" s="18">
+        <v>0.4761904761904762</v>
+      </c>
+      <c r="AS9" s="17"/>
+      <c r="AT9" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="AW9" s="17">
+        <v>1</v>
+      </c>
+      <c r="AX9" s="18">
+        <v>0.04761904761904762</v>
+      </c>
+      <c r="AY9" s="17">
+        <v>5</v>
+      </c>
+      <c r="AZ9" s="17">
+        <v>3</v>
+      </c>
+      <c r="BA9" s="18">
+        <v>0.6666666666666666</v>
+      </c>
+      <c r="BB9" s="18">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="BU9" s="17" t="s">
+        <v>191</v>
+      </c>
+      <c r="BV9" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="BW9" s="17" t="s">
+        <v>199</v>
+      </c>
+      <c r="BX9" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY9" s="17"/>
+    </row>
+    <row r="10" spans="1:77" ht="40" customHeight="1">
+      <c r="A10" s="17" t="s">
+        <v>209</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>217</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H10" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="I10" s="17">
+        <v>1032</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17">
+        <v>0</v>
+      </c>
+      <c r="L10" s="18">
+        <v>0.08261948602994156</v>
+      </c>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17">
+        <v>0</v>
+      </c>
+      <c r="O10" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P10" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="R10" s="19">
+        <v>43336</v>
+      </c>
+      <c r="S10" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="T10" s="17">
+        <v>28</v>
+      </c>
+      <c r="U10" s="17" t="s">
+        <v>221</v>
+      </c>
+      <c r="V10" s="17">
+        <v>11</v>
+      </c>
+      <c r="W10" s="18">
+        <v>0.3928571428571428</v>
+      </c>
+      <c r="X10" s="17"/>
+      <c r="Y10" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="17"/>
+      <c r="AB10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="17"/>
+      <c r="AE10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="17"/>
+      <c r="AH10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ10" s="17"/>
+      <c r="AK10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM10" s="17"/>
+      <c r="AN10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP10" s="17"/>
+      <c r="AQ10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS10" s="17"/>
+      <c r="AT10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV10" s="17"/>
+      <c r="AW10" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX10" s="18">
+        <v>0</v>
+      </c>
+      <c r="AY10" s="17">
+        <v>6</v>
+      </c>
+      <c r="AZ10" s="17">
+        <v>5</v>
+      </c>
+      <c r="BA10" s="18">
+        <v>0.5</v>
+      </c>
+      <c r="BB10" s="18">
+        <v>0.3</v>
+      </c>
+      <c r="BU10" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="BV10" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="BW10" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="BX10" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY10" s="17"/>
+    </row>
+    <row r="11" spans="1:77" ht="40" customHeight="1">
+      <c r="A11" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>227</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="17" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>231</v>
+      </c>
+      <c r="I11" s="17">
+        <v>1275</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17">
+        <v>2</v>
+      </c>
+      <c r="L11" s="18">
+        <v>0.1022336081979025</v>
+      </c>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17">
+        <v>0</v>
+      </c>
+      <c r="O11" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="P11" s="17">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="R11" s="19">
+        <v>43335</v>
+      </c>
+      <c r="S11" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="T11" s="17">
+        <v>25</v>
+      </c>
+      <c r="U11" s="17" t="s">
+        <v>234</v>
+      </c>
+      <c r="V11" s="17">
+        <v>3</v>
+      </c>
+      <c r="W11" s="18">
+        <v>0.12</v>
+      </c>
+      <c r="X11" s="17"/>
+      <c r="Y11" s="17">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="17"/>
+      <c r="AB11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AD11" s="17"/>
+      <c r="AE11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AF11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="17"/>
+      <c r="AH11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AI11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AJ11" s="17"/>
+      <c r="AK11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AL11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AM11" s="17"/>
+      <c r="AN11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AO11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AP11" s="17"/>
+      <c r="AQ11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AR11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AS11" s="17"/>
+      <c r="AT11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AU11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AV11" s="17"/>
+      <c r="AW11" s="17">
+        <v>0</v>
+      </c>
+      <c r="AX11" s="18">
+        <v>0</v>
+      </c>
+      <c r="AY11" s="17"/>
+      <c r="AZ11" s="17"/>
+      <c r="BA11" s="18"/>
+      <c r="BB11" s="18">
+        <v>0.1818181818181818</v>
+      </c>
+      <c r="BU11" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="BV11" s="17" t="s">
+        <v>232</v>
+      </c>
+      <c r="BW11" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="BX11" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="BY11" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="2" width="50.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="17" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="17" t="s">
+        <v>237</v>
+      </c>
+      <c r="B3">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="17" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="18">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="B7" s="18">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="B8" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="17" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" s="17" t="s">
+        <v>244</v>
+      </c>
+      <c r="B10" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="B11" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="17" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="17" t="s">
+        <v>247</v>
+      </c>
+      <c r="B13" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="17" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="17" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="17" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="17" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="17" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="17" t="s">
+        <v>254</v>
+      </c>
+      <c r="B20" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="17" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="17" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="17" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="17" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="17" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="17" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="17" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="17" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="17" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="17" t="s">
+        <v>266</v>
+      </c>
+      <c r="B32" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="17" t="s">
+        <v>267</v>
+      </c>
+      <c r="B33" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="17" t="s">
+        <v>268</v>
+      </c>
+      <c r="B34" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="B35" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="17" t="s">
+        <v>270</v>
+      </c>
+      <c r="B36" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="B37" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="17" t="s">
+        <v>272</v>
+      </c>
+      <c r="B38" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="17" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="B40" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="17" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="17" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="17" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="B44">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="B45" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="17" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="17" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="17" t="s">
+        <v>282</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>